<commit_message>
reportes show e info, contratos correciones
</commit_message>
<xml_diff>
--- a/importadores/simcard_claro.xlsx
+++ b/importadores/simcard_claro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp3\htdocs\talentus\importadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B689C6C6-5DA6-46AE-8450-38A6022C8190}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED34FC5-2896-44BC-B37B-8BE692FA484A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="1561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1214">
   <si>
     <t>numero</t>
   </si>
@@ -3645,1069 +3645,28 @@
     <t>Claro</t>
   </si>
   <si>
-    <t>8951101632059530497</t>
-  </si>
-  <si>
-    <t>8951101639163531956</t>
-  </si>
-  <si>
-    <t>8951101639146772479</t>
-  </si>
-  <si>
-    <t>8951101632059530794</t>
-  </si>
-  <si>
-    <t>8951101632059530786</t>
-  </si>
-  <si>
-    <t>8951101632059530778</t>
-  </si>
-  <si>
-    <t>8951101632059530760</t>
-  </si>
-  <si>
-    <t>8951101632059530752</t>
-  </si>
-  <si>
-    <t>8951101632059530489</t>
-  </si>
-  <si>
-    <t>8951101632059530463</t>
-  </si>
-  <si>
-    <t>8951101632059530455</t>
-  </si>
-  <si>
-    <t>8951101632059530448</t>
-  </si>
-  <si>
-    <t>8951101632059530430</t>
-  </si>
-  <si>
-    <t>8951101632059530422</t>
-  </si>
-  <si>
-    <t>8951101632059530414</t>
-  </si>
-  <si>
-    <t>8951101632059531214</t>
-  </si>
-  <si>
-    <t>8951101632059531206</t>
-  </si>
-  <si>
-    <t>8951101630203715758</t>
-  </si>
-  <si>
-    <t>8951101632059531180</t>
-  </si>
-  <si>
-    <t>8951101632059531172</t>
-  </si>
-  <si>
-    <t>8951101632059531354</t>
-  </si>
-  <si>
-    <t>8951101632059531347</t>
-  </si>
-  <si>
-    <t>8951101632059531339</t>
-  </si>
-  <si>
-    <t>8951101632634954725</t>
-  </si>
-  <si>
-    <t>8951101632059531321</t>
-  </si>
-  <si>
-    <t>8951101632059531305</t>
-  </si>
-  <si>
-    <t>8951101632059531297</t>
-  </si>
-  <si>
-    <t>8951101632059531289</t>
-  </si>
-  <si>
-    <t>8951101632059531271</t>
-  </si>
-  <si>
-    <t>8951101632059531263</t>
-  </si>
-  <si>
-    <t>8951101632059531255</t>
-  </si>
-  <si>
-    <t>8951101632059531248</t>
-  </si>
-  <si>
-    <t>8951101632059531230</t>
-  </si>
-  <si>
-    <t>8951101632059531222</t>
-  </si>
-  <si>
-    <t>8951100312213610474</t>
-  </si>
-  <si>
-    <t>8951101632226742249</t>
-  </si>
-  <si>
-    <t>8951101632226742256</t>
-  </si>
-  <si>
-    <t>8951101639146772529</t>
-  </si>
-  <si>
-    <t>8951101632226742272</t>
-  </si>
-  <si>
-    <t>8951101639297673112</t>
-  </si>
-  <si>
-    <t>8951101632226742280</t>
-  </si>
-  <si>
-    <t>8951101632226742298</t>
-  </si>
-  <si>
-    <t>8951101632226742306</t>
-  </si>
-  <si>
-    <t>8951101632226742314</t>
-  </si>
-  <si>
-    <t>8951101630203715832</t>
-  </si>
-  <si>
-    <t>913949534</t>
-  </si>
-  <si>
-    <t>8951101630101839924</t>
-  </si>
-  <si>
-    <t>914344570</t>
-  </si>
-  <si>
-    <t>8951101630383929153</t>
-  </si>
-  <si>
-    <t>914344579</t>
-  </si>
-  <si>
-    <t>8951101630685915231</t>
-  </si>
-  <si>
-    <t>914344597</t>
-  </si>
-  <si>
-    <t>8951101639436110711</t>
-  </si>
-  <si>
-    <t>914344599</t>
-  </si>
-  <si>
-    <t>8951101639575343685</t>
-  </si>
-  <si>
-    <t>914344669</t>
-  </si>
-  <si>
-    <t>8951101630384025738</t>
-  </si>
-  <si>
-    <t>914344700</t>
-  </si>
-  <si>
-    <t>8951101639436110539</t>
-  </si>
-  <si>
-    <t>914344873</t>
-  </si>
-  <si>
-    <t>8951101639498060531</t>
-  </si>
-  <si>
-    <t>914345064</t>
-  </si>
-  <si>
-    <t>8951101632645961487</t>
-  </si>
-  <si>
-    <t>914345134</t>
-  </si>
-  <si>
-    <t>8951101632645961636</t>
-  </si>
-  <si>
-    <t>914345216</t>
-  </si>
-  <si>
-    <t>8951101639575380455</t>
-  </si>
-  <si>
-    <t>932691461</t>
-  </si>
-  <si>
-    <t>8951101639436132368</t>
-  </si>
-  <si>
-    <t>932691462</t>
-  </si>
-  <si>
-    <t>8951101639436132376</t>
-  </si>
-  <si>
-    <t>932691472</t>
-  </si>
-  <si>
-    <t>8951101630541810469</t>
-  </si>
-  <si>
-    <t>932691478</t>
-  </si>
-  <si>
-    <t>8951101639436132392</t>
-  </si>
-  <si>
-    <t>932691479</t>
-  </si>
-  <si>
-    <t>8951101639436132400</t>
-  </si>
-  <si>
-    <t>932691485</t>
-  </si>
-  <si>
-    <t>8951101639436132418</t>
-  </si>
-  <si>
-    <t>932691494</t>
-  </si>
-  <si>
-    <t>8951101639436132426</t>
-  </si>
-  <si>
-    <t>932691516</t>
-  </si>
-  <si>
-    <t>8951101639436110679</t>
-  </si>
-  <si>
-    <t>932691521</t>
-  </si>
-  <si>
-    <t>8951101639436132442</t>
-  </si>
-  <si>
-    <t>932691530</t>
-  </si>
-  <si>
-    <t>8951101630685915207</t>
-  </si>
-  <si>
-    <t>932692045</t>
-  </si>
-  <si>
-    <t>8951101639588395946</t>
-  </si>
-  <si>
-    <t>932692051</t>
-  </si>
-  <si>
-    <t>8951101639489629344</t>
-  </si>
-  <si>
-    <t>932692068</t>
-  </si>
-  <si>
-    <t>8951101630541810535</t>
-  </si>
-  <si>
-    <t>932692091</t>
-  </si>
-  <si>
-    <t>8951101630388660969</t>
-  </si>
-  <si>
-    <t>932692119</t>
-  </si>
-  <si>
-    <t>8951101639575380539</t>
-  </si>
-  <si>
-    <t>932692125</t>
-  </si>
-  <si>
-    <t>8951101632645961511</t>
-  </si>
-  <si>
-    <t>932692141</t>
-  </si>
-  <si>
-    <t>8951101639498060481</t>
-  </si>
-  <si>
-    <t>932692150</t>
-  </si>
-  <si>
-    <t>8951101639489629294</t>
-  </si>
-  <si>
-    <t>932692153</t>
-  </si>
-  <si>
-    <t>8951101639792782244</t>
-  </si>
-  <si>
-    <t>932692201</t>
-  </si>
-  <si>
-    <t>8951101630608515472</t>
-  </si>
-  <si>
-    <t>940368155</t>
-  </si>
-  <si>
-    <t>8951101632458592486</t>
-  </si>
-  <si>
-    <t>940368261</t>
-  </si>
-  <si>
-    <t>8951101632645961446</t>
-  </si>
-  <si>
-    <t>940368424</t>
-  </si>
-  <si>
-    <t>8951101630685915314</t>
-  </si>
-  <si>
-    <t>940368791</t>
-  </si>
-  <si>
-    <t>8951101639489636034</t>
-  </si>
-  <si>
-    <t>940368934</t>
-  </si>
-  <si>
-    <t>8951101639792782228</t>
-  </si>
-  <si>
-    <t>940369094</t>
-  </si>
-  <si>
-    <t>8951101639588396050</t>
-  </si>
-  <si>
-    <t>940408864</t>
-  </si>
-  <si>
-    <t>8951101630685915223</t>
-  </si>
-  <si>
-    <t>940409007</t>
-  </si>
-  <si>
-    <t>8951101639575380380</t>
-  </si>
-  <si>
-    <t>940409107</t>
-  </si>
-  <si>
-    <t>8951101639588396001</t>
-  </si>
-  <si>
-    <t>940409386</t>
-  </si>
-  <si>
-    <t>8951101630597875168</t>
-  </si>
-  <si>
-    <t>940457356</t>
-  </si>
-  <si>
-    <t>8951101639509267133</t>
-  </si>
-  <si>
-    <t>940457429</t>
-  </si>
-  <si>
-    <t>8951101639504128546</t>
-  </si>
-  <si>
-    <t>940458010</t>
-  </si>
-  <si>
-    <t>8951101632645961685</t>
-  </si>
-  <si>
-    <t>940458014</t>
-  </si>
-  <si>
-    <t>8951101639509267166</t>
-  </si>
-  <si>
-    <t>940458362</t>
-  </si>
-  <si>
-    <t>8951101632634954758</t>
-  </si>
-  <si>
-    <t>944052639</t>
-  </si>
-  <si>
-    <t>8951101639418878368</t>
-  </si>
-  <si>
-    <t>944052735</t>
-  </si>
-  <si>
-    <t>8951101639418878434</t>
-  </si>
-  <si>
-    <t>944052780</t>
-  </si>
-  <si>
-    <t>8951101639418878384</t>
-  </si>
-  <si>
-    <t>944053793</t>
-  </si>
-  <si>
-    <t>8951101639489629310</t>
-  </si>
-  <si>
-    <t>944054006</t>
-  </si>
-  <si>
-    <t>8951101632357690761</t>
-  </si>
-  <si>
-    <t>944054018</t>
-  </si>
-  <si>
-    <t>8951101632357690779</t>
-  </si>
-  <si>
-    <t>944054126</t>
-  </si>
-  <si>
-    <t>8951101632357690787</t>
-  </si>
-  <si>
-    <t>944054236</t>
-  </si>
-  <si>
-    <t>8951101639509267158</t>
-  </si>
-  <si>
-    <t>944054279</t>
-  </si>
-  <si>
-    <t>8951101639792782442</t>
-  </si>
-  <si>
-    <t>944054618</t>
-  </si>
-  <si>
-    <t>8951101630388660316</t>
-  </si>
-  <si>
-    <t>944058911</t>
-  </si>
-  <si>
-    <t>8951101639408788734</t>
-  </si>
-  <si>
-    <t>944059488</t>
-  </si>
-  <si>
-    <t>8951101639491136544</t>
-  </si>
-  <si>
-    <t>944059608</t>
-  </si>
-  <si>
-    <t>8951101639792782483</t>
-  </si>
-  <si>
-    <t>944060145</t>
-  </si>
-  <si>
-    <t>8951101630388660522</t>
-  </si>
-  <si>
-    <t>944060734</t>
-  </si>
-  <si>
-    <t>8951101639588395961</t>
-  </si>
-  <si>
-    <t>944061308</t>
-  </si>
-  <si>
-    <t>944061418</t>
-  </si>
-  <si>
-    <t>8951101639504128470</t>
-  </si>
-  <si>
-    <t>944061944</t>
-  </si>
-  <si>
-    <t>8951101630388660563</t>
-  </si>
-  <si>
-    <t>944062506</t>
-  </si>
-  <si>
-    <t>8951101632458592403</t>
-  </si>
-  <si>
-    <t>944062575</t>
-  </si>
-  <si>
-    <t>8951101639792782418</t>
-  </si>
-  <si>
-    <t>944071859</t>
-  </si>
-  <si>
-    <t>8951101639436110760</t>
-  </si>
-  <si>
-    <t>944072193</t>
-  </si>
-  <si>
-    <t>8951101632645961545</t>
-  </si>
-  <si>
-    <t>944072442</t>
-  </si>
-  <si>
-    <t>8951101632426844878</t>
-  </si>
-  <si>
-    <t>944073044</t>
-  </si>
-  <si>
-    <t>8951101639491955166</t>
-  </si>
-  <si>
-    <t>944073619</t>
-  </si>
-  <si>
-    <t>8951101630685915249</t>
-  </si>
-  <si>
-    <t>944073661</t>
-  </si>
-  <si>
-    <t>8951101639411674921</t>
-  </si>
-  <si>
-    <t>944073677</t>
-  </si>
-  <si>
-    <t>8951101630608444350</t>
-  </si>
-  <si>
-    <t>944073773</t>
-  </si>
-  <si>
-    <t>8951101630388660910</t>
-  </si>
-  <si>
-    <t>944074232</t>
-  </si>
-  <si>
-    <t>8951101630388660928</t>
-  </si>
-  <si>
-    <t>944074233</t>
-  </si>
-  <si>
-    <t>8951101630597875135</t>
-  </si>
-  <si>
-    <t>944074911</t>
-  </si>
-  <si>
-    <t>8951101632426844803</t>
-  </si>
-  <si>
-    <t>944075542</t>
-  </si>
-  <si>
-    <t>8951101632484662642</t>
-  </si>
-  <si>
-    <t>944075837</t>
-  </si>
-  <si>
-    <t>8951101639408788635</t>
-  </si>
-  <si>
-    <t>944076895</t>
-  </si>
-  <si>
-    <t>8951101630685915264</t>
-  </si>
-  <si>
-    <t>944077269</t>
-  </si>
-  <si>
-    <t>8951101632066570114</t>
-  </si>
-  <si>
-    <t>944077819</t>
-  </si>
-  <si>
-    <t>8951101639438134529</t>
-  </si>
-  <si>
-    <t>944077848</t>
-  </si>
-  <si>
-    <t>8951101630685915413</t>
-  </si>
-  <si>
-    <t>944078263</t>
-  </si>
-  <si>
-    <t>8951101630388661025</t>
-  </si>
-  <si>
-    <t>944078380</t>
-  </si>
-  <si>
-    <t>8951101630388660886</t>
-  </si>
-  <si>
-    <t>944078466</t>
-  </si>
-  <si>
-    <t>8951101639408788585</t>
-  </si>
-  <si>
-    <t>8951101630383929161</t>
-  </si>
-  <si>
-    <t>944740306</t>
-  </si>
-  <si>
-    <t>8951101630608444327</t>
-  </si>
-  <si>
-    <t>944740430</t>
-  </si>
-  <si>
-    <t>8951101630541807754</t>
-  </si>
-  <si>
-    <t>944740526</t>
-  </si>
-  <si>
-    <t>8951101639588395813</t>
-  </si>
-  <si>
-    <t>944740609</t>
-  </si>
-  <si>
-    <t>8951101632634991693</t>
-  </si>
-  <si>
-    <t>944740818</t>
-  </si>
-  <si>
-    <t>8951101632458592353</t>
-  </si>
-  <si>
-    <t>944741217</t>
-  </si>
-  <si>
-    <t>8951101630519878605</t>
-  </si>
-  <si>
-    <t>944741364</t>
-  </si>
-  <si>
-    <t>8951101639792782392</t>
-  </si>
-  <si>
-    <t>944741526</t>
-  </si>
-  <si>
-    <t>8951101639588395821</t>
-  </si>
-  <si>
-    <t>944741754</t>
-  </si>
-  <si>
-    <t>8951101630685915330</t>
-  </si>
-  <si>
-    <t>8951101632348827951</t>
-  </si>
-  <si>
-    <t>8951101632348827977</t>
-  </si>
-  <si>
-    <t>8951101632348827993</t>
-  </si>
-  <si>
-    <t>8951101632357698533</t>
-  </si>
-  <si>
-    <t>8951101632348828017</t>
-  </si>
-  <si>
-    <t>8951101632348828025</t>
-  </si>
-  <si>
-    <t>8951101632357690845</t>
-  </si>
-  <si>
-    <t>8951101632426844795</t>
-  </si>
-  <si>
-    <t>8951101630108171958</t>
-  </si>
-  <si>
-    <t>8951101630108171966</t>
-  </si>
-  <si>
-    <t>949700853</t>
-  </si>
-  <si>
-    <t>8951101630388660241</t>
-  </si>
-  <si>
-    <t>8951101631322585221</t>
-  </si>
-  <si>
-    <t>949701106</t>
-  </si>
-  <si>
-    <t>8951101639163592289</t>
-  </si>
-  <si>
-    <t>8951101631322585239</t>
-  </si>
-  <si>
-    <t>8951101632350142299</t>
-  </si>
-  <si>
-    <t>949707715</t>
-  </si>
-  <si>
-    <t>8951101631322585213</t>
-  </si>
-  <si>
-    <t>8951101630330776343</t>
-  </si>
-  <si>
-    <t>8951101630330776350</t>
-  </si>
-  <si>
-    <t>8951101630330776368</t>
-  </si>
-  <si>
-    <t>8951101630519878548</t>
-  </si>
-  <si>
-    <t>8951101630388660506</t>
-  </si>
-  <si>
-    <t>8951101639158641927</t>
-  </si>
-  <si>
-    <t>958969013</t>
-  </si>
-  <si>
-    <t>8951101632347503538</t>
-  </si>
-  <si>
-    <t>958969350</t>
-  </si>
-  <si>
-    <t>8951101632347503512</t>
-  </si>
-  <si>
-    <t>958969366</t>
-  </si>
-  <si>
-    <t>8951101632347503520</t>
-  </si>
-  <si>
-    <t>8951101639158641968</t>
-  </si>
-  <si>
-    <t>8951101639158641976</t>
-  </si>
-  <si>
-    <t>8951101639297673187</t>
-  </si>
-  <si>
-    <t>958969494</t>
-  </si>
-  <si>
-    <t>8951101639163592321</t>
-  </si>
-  <si>
-    <t>8951101639158642008</t>
-  </si>
-  <si>
-    <t>8951101639158642016</t>
-  </si>
-  <si>
-    <t>8951101639158642024</t>
-  </si>
-  <si>
-    <t>8951101639158642040</t>
-  </si>
-  <si>
-    <t>8951101639158642057</t>
-  </si>
-  <si>
-    <t>8951101639158642065</t>
-  </si>
-  <si>
-    <t>8951101639158642073</t>
-  </si>
-  <si>
-    <t>8951101639575343701</t>
-  </si>
-  <si>
-    <t>8951101632347503439</t>
-  </si>
-  <si>
-    <t>8951101639575380331</t>
-  </si>
-  <si>
-    <t>8951101630108171917</t>
-  </si>
-  <si>
-    <t>8951101630108171925</t>
-  </si>
-  <si>
-    <t>8951101630108171933</t>
-  </si>
-  <si>
-    <t>8951101632059533459</t>
-  </si>
-  <si>
-    <t>8951101632059533442</t>
-  </si>
-  <si>
-    <t>8951101632059533160</t>
-  </si>
-  <si>
-    <t>8951101632059533152</t>
-  </si>
-  <si>
-    <t>8951101632059533350</t>
-  </si>
-  <si>
-    <t>8951101632059533277</t>
-  </si>
-  <si>
-    <t>8951101632059533186</t>
-  </si>
-  <si>
-    <t>8951101632059533178</t>
-  </si>
-  <si>
-    <t>8951101630108171891</t>
-  </si>
-  <si>
-    <t>8951101639489629153</t>
-  </si>
-  <si>
-    <t>8951101632645961438</t>
-  </si>
-  <si>
-    <t>8951101639504128579</t>
-  </si>
-  <si>
-    <t>8951101630597875101</t>
-  </si>
-  <si>
-    <t>8951101639308887347</t>
-  </si>
-  <si>
-    <t>8951101632347503371</t>
-  </si>
-  <si>
-    <t>8951101630108171909</t>
-  </si>
-  <si>
-    <t>8951101630685915348</t>
-  </si>
-  <si>
-    <t>8951101632347503413</t>
-  </si>
-  <si>
-    <t>8951101639411674939</t>
-  </si>
-  <si>
-    <t>8951101639163532004</t>
-  </si>
-  <si>
-    <t>8951101632347503470</t>
-  </si>
-  <si>
-    <t>8951101639297673104</t>
-  </si>
-  <si>
-    <t>8951101630597875143</t>
-  </si>
-  <si>
-    <t>8951101639498260941</t>
-  </si>
-  <si>
-    <t>8951101639146772503</t>
-  </si>
-  <si>
-    <t>8951101632624048801</t>
-  </si>
-  <si>
-    <t>8951101639504128637</t>
-  </si>
-  <si>
-    <t>8951101632645961560</t>
-  </si>
-  <si>
-    <t>8951101632347503421</t>
-  </si>
-  <si>
-    <t>8951101639297673070</t>
-  </si>
-  <si>
-    <t>8951101630330774850</t>
-  </si>
-  <si>
-    <t>8951101639297673120</t>
-  </si>
-  <si>
-    <t>8951101630330774876</t>
-  </si>
-  <si>
-    <t>8951101632286371574</t>
-  </si>
-  <si>
-    <t>8951101630330774892</t>
-  </si>
-  <si>
-    <t>8951101631322585395</t>
-  </si>
-  <si>
-    <t>8951101631322585379</t>
-  </si>
-  <si>
-    <t>8951101630330774934</t>
-  </si>
-  <si>
-    <t>8951101630330775188</t>
-  </si>
-  <si>
-    <t>8951101630330775196</t>
-  </si>
-  <si>
-    <t>8951101632347503462</t>
-  </si>
-  <si>
-    <t>8951101630330775220</t>
-  </si>
-  <si>
-    <t>8951101632634991552</t>
-  </si>
-  <si>
-    <t>8951101639575380489</t>
-  </si>
-  <si>
-    <t>8951101632634991719</t>
-  </si>
-  <si>
-    <t>8951101631322585247</t>
-  </si>
-  <si>
-    <t>8951101632347607149</t>
-  </si>
-  <si>
-    <t>8951101632634991701</t>
-  </si>
-  <si>
-    <t>8951101639436013154</t>
-  </si>
-  <si>
-    <t>8951101639408688892</t>
-  </si>
-  <si>
-    <t>8951101639792782400</t>
-  </si>
-  <si>
-    <t>8951101639575343842</t>
-  </si>
-  <si>
-    <t>8951101632458592361</t>
-  </si>
-  <si>
-    <t>8951101639504128447</t>
-  </si>
-  <si>
-    <t>958178033</t>
-  </si>
-  <si>
-    <t>8951101630330775238</t>
-  </si>
-  <si>
-    <t>958955294</t>
-  </si>
-  <si>
-    <t>8951101639158641612</t>
-  </si>
-  <si>
-    <t>958955309</t>
-  </si>
-  <si>
-    <t>8951101639158641620</t>
-  </si>
-  <si>
-    <t>8951101632458592379</t>
-  </si>
-  <si>
-    <t>8951101632347503397</t>
-  </si>
-  <si>
-    <t>8951101632426844936</t>
-  </si>
-  <si>
-    <t>8951101632458592395</t>
-  </si>
-  <si>
-    <t>8951101639436110570</t>
-  </si>
-  <si>
-    <t>8951101639498260842</t>
-  </si>
-  <si>
-    <t>8951101632634991735</t>
-  </si>
-  <si>
-    <t>8951101630531467635</t>
-  </si>
-  <si>
-    <t>8951101639163592313</t>
-  </si>
-  <si>
-    <t>8951101630608515399</t>
-  </si>
-  <si>
-    <t>8951101632634991586</t>
+    <t>987814757</t>
+  </si>
+  <si>
+    <t>8951101639590982228</t>
+  </si>
+  <si>
+    <t>987815012</t>
+  </si>
+  <si>
+    <t>8951101639590982236</t>
+  </si>
+  <si>
+    <t>987816560</t>
+  </si>
+  <si>
+    <t>8951101639590982244</t>
+  </si>
+  <si>
+    <t>987816634</t>
+  </si>
+  <si>
+    <t>8951101630608444467</t>
   </si>
 </sst>
 </file>
@@ -4717,7 +3676,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4858,6 +3817,10 @@
       <sz val="8"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Trebuchet MS"/>
     </font>
   </fonts>
   <fills count="33">
@@ -5222,7 +4185,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5231,13 +4194,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5563,10 +4520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1043"/>
+  <dimension ref="A1:C629"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A885" workbookViewId="0">
-      <selection activeCell="D913" sqref="D913"/>
+    <sheetView tabSelected="1" topLeftCell="A611" workbookViewId="0">
+      <selection activeCell="B624" sqref="B624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12408,3378 +11365,90 @@
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A622" s="4" t="s">
-        <v>3</v>
+        <v>1206</v>
       </c>
       <c r="B622" s="4" t="s">
-        <v>4</v>
+        <v>1207</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1205</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A623" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B623" s="5" t="s">
+      <c r="A623" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B623" s="4" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A624" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B624" s="4" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B625" s="4" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" s="4" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A624" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B624" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A625" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B625" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A626" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B626" s="5" t="s">
+      <c r="B626" s="4" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A627" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B627" s="6">
-        <v>8.9511016391635302E+18</v>
-      </c>
-    </row>
-    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A628" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B628" s="5" t="s">
+      <c r="C626" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" s="4" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A629" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B629" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A630" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B630" s="5" t="s">
+      <c r="B627" s="4" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A631" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B631" s="5" t="s">
+      <c r="C627" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A628" s="4" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A632" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B632" s="5" t="s">
+      <c r="B628" s="4" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A633" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B633" s="5" t="s">
+      <c r="C628" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" s="4" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A634" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B634" s="5" t="s">
+      <c r="B629" s="4" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A635" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B635" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A636" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B636" s="5" t="s">
-        <v>1214</v>
-      </c>
-    </row>
-    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A637" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B637" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A638" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B638" s="5" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A639" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B639" s="5" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A640" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B640" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A641" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B641" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A642" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B642" s="5" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A643" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B643" s="5" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A644" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B644" s="5" t="s">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A645" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B645" s="5" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A646" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B646" s="5" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A647" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B647" s="5" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A648" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B648" s="5" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A649" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B649" s="5" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A650" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B650" s="5" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A651" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B651" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A652" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B652" s="5" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A653" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B653" s="5" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A654" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B654" s="5" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A655" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B655" s="5" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A656" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B656" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A657" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B657" s="5" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A658" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B658" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A659" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B659" s="5" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A660" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B660" s="5" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A661" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B661" s="5" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A662" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B662" s="5" t="s">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A663" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B663" s="5" t="s">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A664" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B664" s="5" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A665" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B665" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A666" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B666" s="5" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A667" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B667" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A668" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B668" s="5" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A669" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B669" s="5" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A670" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B670" s="5" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A671" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B671" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A672" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B672" s="5" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A673" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B673" s="5" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A674" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B674" s="5" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A675" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B675" s="5" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A676" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B676" s="5" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A677" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B677" s="5" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A678" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B678" s="5" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A679" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B679" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A680" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B680" s="5" t="s">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A681" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B681" s="5" t="s">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A682" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B682" s="5" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A683" s="5" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B683" s="5" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A684" s="5" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B684" s="5" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A685" s="5" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B685" s="5" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A686" s="5" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B686" s="5" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="5" t="s">
-        <v>1259</v>
-      </c>
-      <c r="B687" s="5" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" s="5" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B688" s="5" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A689" s="5" t="s">
-        <v>1263</v>
-      </c>
-      <c r="B689" s="5" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A690" s="5" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B690" s="5" t="s">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" s="5" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B691" s="5" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="5" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B692" s="5" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A693" s="5" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B693" s="5" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A694" s="5" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B694" s="5" t="s">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A695" s="5" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B695" s="5" t="s">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A696" s="5" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B696" s="5" t="s">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" s="5" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B697" s="5" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="5" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B698" s="5" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" s="5" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B699" s="5" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A700" s="5" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B700" s="5" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A701" s="5" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B701" s="5" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" s="5" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B702" s="5" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="5" t="s">
-        <v>1291</v>
-      </c>
-      <c r="B703" s="5" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" s="5" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B704" s="5" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" s="5" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B705" s="5" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" s="5" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B706" s="5" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A707" s="5" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B707" s="5" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="5" t="s">
-        <v>1301</v>
-      </c>
-      <c r="B708" s="5" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" s="5" t="s">
-        <v>1303</v>
-      </c>
-      <c r="B709" s="5" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A710" s="5" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B710" s="5" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A711" s="5" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B711" s="5" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A712" s="5" t="s">
-        <v>1309</v>
-      </c>
-      <c r="B712" s="5" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="5" t="s">
-        <v>1311</v>
-      </c>
-      <c r="B713" s="5" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A714" s="5" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B714" s="5" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A715" s="5" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B715" s="5" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A716" s="5" t="s">
-        <v>1317</v>
-      </c>
-      <c r="B716" s="5" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A717" s="5" t="s">
-        <v>1319</v>
-      </c>
-      <c r="B717" s="5" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="5" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B718" s="5" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A719" s="5" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B719" s="5" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A720" s="5" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B720" s="5" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A721" s="5" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B721" s="5" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" s="5" t="s">
-        <v>1329</v>
-      </c>
-      <c r="B722" s="5" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="5" t="s">
-        <v>1331</v>
-      </c>
-      <c r="B723" s="5" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A724" s="5" t="s">
-        <v>1333</v>
-      </c>
-      <c r="B724" s="5" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A725" s="5" t="s">
-        <v>1335</v>
-      </c>
-      <c r="B725" s="5" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A726" s="5" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B726" s="5" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A727" s="5" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B727" s="5" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="5" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B728" s="5" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A729" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B729" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A730" s="5" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B730" s="5" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A731" s="5" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B731" s="5" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A732" s="5" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B732" s="5" t="s">
-        <v>1348</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A733" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="B733" s="5" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A734" s="5" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B734" s="5" t="s">
-        <v>1352</v>
-      </c>
-    </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A735" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B735" s="5" t="s">
-        <v>1354</v>
-      </c>
-    </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A736" s="5" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B736" s="5" t="s">
-        <v>1356</v>
-      </c>
-    </row>
-    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="5" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B737" s="5" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A738" s="5" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B738" s="5" t="s">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A739" s="5" t="s">
-        <v>1361</v>
-      </c>
-      <c r="B739" s="5" t="s">
-        <v>1362</v>
-      </c>
-    </row>
-    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A740" s="5" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B740" s="5" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A741" s="5" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B741" s="5" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A742" s="5" t="s">
-        <v>1367</v>
-      </c>
-      <c r="B742" s="5" t="s">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A743" s="5" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B743" s="5" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A744" s="5" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B744" s="5" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A745" s="5" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B745" s="5" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="5" t="s">
-        <v>1374</v>
-      </c>
-      <c r="B746" s="5" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" s="5" t="s">
-        <v>1376</v>
-      </c>
-      <c r="B747" s="5" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A748" s="5" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B748" s="5" t="s">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A749" s="5" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B749" s="5" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A750" s="5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B750" s="5" t="s">
-        <v>1383</v>
-      </c>
-    </row>
-    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A751" s="5" t="s">
-        <v>1384</v>
-      </c>
-      <c r="B751" s="5" t="s">
-        <v>1385</v>
-      </c>
-    </row>
-    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A752" s="5" t="s">
-        <v>1386</v>
-      </c>
-      <c r="B752" s="5" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A753" s="5" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B753" s="5" t="s">
-        <v>1389</v>
-      </c>
-    </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A754" s="5" t="s">
-        <v>1390</v>
-      </c>
-      <c r="B754" s="5" t="s">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="5" t="s">
-        <v>1392</v>
-      </c>
-      <c r="B755" s="5" t="s">
-        <v>1393</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" s="5" t="s">
-        <v>1394</v>
-      </c>
-      <c r="B756" s="5" t="s">
-        <v>1395</v>
-      </c>
-    </row>
-    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A757" s="5" t="s">
-        <v>1396</v>
-      </c>
-      <c r="B757" s="5" t="s">
-        <v>1397</v>
-      </c>
-    </row>
-    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A758" s="5" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B758" s="5" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A759" s="5" t="s">
-        <v>1400</v>
-      </c>
-      <c r="B759" s="5" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A760" s="5" t="s">
-        <v>1402</v>
-      </c>
-      <c r="B760" s="5" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A761" s="5" t="s">
-        <v>1404</v>
-      </c>
-      <c r="B761" s="5" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A762" s="5" t="s">
-        <v>1406</v>
-      </c>
-      <c r="B762" s="5" t="s">
-        <v>1407</v>
-      </c>
-    </row>
-    <row r="763" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A763" s="5" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B763" s="5" t="s">
-        <v>1409</v>
-      </c>
-    </row>
-    <row r="764" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A764" s="5" t="s">
-        <v>1410</v>
-      </c>
-      <c r="B764" s="5" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="765" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A765" s="5" t="s">
-        <v>1412</v>
-      </c>
-      <c r="B765" s="5" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="766" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A766" s="5" t="s">
-        <v>1414</v>
-      </c>
-      <c r="B766" s="5" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="767" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A767" s="5" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B767" s="5" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="768" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A768" s="5" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B768" s="5" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="769" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A769" s="5" t="s">
-        <v>1420</v>
-      </c>
-      <c r="B769" s="5" t="s">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="770" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A770" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B770" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="771" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A771" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B771" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="772" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A772" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B772" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="773" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A773" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B773" s="5" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="774" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A774" s="5" t="s">
-        <v>1423</v>
-      </c>
-      <c r="B774" s="5" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="775" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A775" s="5" t="s">
-        <v>1425</v>
-      </c>
-      <c r="B775" s="5" t="s">
-        <v>1426</v>
-      </c>
-    </row>
-    <row r="776" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A776" s="5" t="s">
-        <v>1427</v>
-      </c>
-      <c r="B776" s="5" t="s">
-        <v>1428</v>
-      </c>
-    </row>
-    <row r="777" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A777" s="5" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B777" s="5" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="778" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A778" s="5" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B778" s="5" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="779" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A779" s="5" t="s">
-        <v>1433</v>
-      </c>
-      <c r="B779" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="780" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A780" s="5" t="s">
-        <v>1435</v>
-      </c>
-      <c r="B780" s="5" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="781" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A781" s="5" t="s">
-        <v>1437</v>
-      </c>
-      <c r="B781" s="5" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A782" s="5" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B782" s="5" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="783" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A783" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B783" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="784" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A784" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B784" s="5" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="785" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A785" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B785" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="786" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A786" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B786" s="5" t="s">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="787" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A787" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B787" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="788" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A788" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B788" s="5" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="789" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A789" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B789" s="5" t="s">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="790" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A790" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B790" s="5" t="s">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="791" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A791" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B791" s="5" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="792" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A792" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="B792" s="5" t="s">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="793" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A793" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B793" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="794" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A794" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B794" s="5" t="s">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="795" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A795" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B795" s="5" t="s">
-        <v>1449</v>
-      </c>
-    </row>
-    <row r="796" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A796" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B796" s="5" t="s">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="797" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A797" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B797" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="798" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A798" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B798" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="799" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A799" s="5" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B799" s="5" t="s">
-        <v>1452</v>
-      </c>
-    </row>
-    <row r="800" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A800" s="5" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B800" s="5" t="s">
-        <v>1453</v>
-      </c>
-    </row>
-    <row r="801" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A801" s="5" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B801" s="5" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="802" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A802" s="5" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B802" s="5" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A803" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B803" s="5" t="s">
-        <v>1457</v>
-      </c>
-    </row>
-    <row r="804" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A804" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B804" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="805" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A805" s="5" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B805" s="5" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="806" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A806" s="5" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B806" s="5" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="807" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A807" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="B807" s="5" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="808" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A808" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B808" s="5" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="809" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A809" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B809" s="5" t="s">
-        <v>1462</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A810" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B810" s="5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="811" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A811" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B811" s="5" t="s">
-        <v>1463</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A812" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="B812" s="5" t="s">
-        <v>1464</v>
-      </c>
-    </row>
-    <row r="813" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A813" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="B813" s="5" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A814" s="5" t="s">
-        <v>1466</v>
-      </c>
-      <c r="B814" s="5" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="815" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A815" s="5" t="s">
-        <v>1468</v>
-      </c>
-      <c r="B815" s="5" t="s">
-        <v>1469</v>
-      </c>
-    </row>
-    <row r="816" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A816" s="5" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B816" s="5" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A817" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="B817" s="5" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A818" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="B818" s="5" t="s">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A819" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B819" s="5" t="s">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A820" s="5" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B820" s="5" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A821" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B821" s="5" t="s">
-        <v>1477</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A822" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B822" s="5" t="s">
-        <v>1478</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A823" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="B823" s="5" t="s">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A824" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B824" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A825" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B825" s="5" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A826" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="B826" s="5" t="s">
-        <v>1481</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A827" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="B827" s="5" t="s">
-        <v>1482</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A828" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B828" s="5" t="s">
-        <v>1483</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A829" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="B829" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A830" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="B830" s="5" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A831" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="B831" s="5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="832" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A832" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B832" s="5" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A833" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="B833" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A834" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="B834" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A835" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B835" s="5" t="s">
-        <v>1484</v>
-      </c>
-    </row>
-    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A836" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B836" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A837" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B837" s="5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A838" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B838" s="5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A839" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B839" s="5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A840" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B840" s="5" t="s">
-        <v>1485</v>
-      </c>
-    </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A841" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B841" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A842" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B842" s="5" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A843" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B843" s="5" t="s">
-        <v>1487</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A844" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B844" s="5" t="s">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A845" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B845" s="5" t="s">
-        <v>1489</v>
-      </c>
-    </row>
-    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A846" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B846" s="5" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A847" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="B847" s="5" t="s">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A848" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="B848" s="5" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A849" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="B849" s="5" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A850" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B850" s="5" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A851" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B851" s="5" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A852" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="B852" s="5" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A853" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="B853" s="5" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A854" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="B854" s="5" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A855" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="B855" s="5" t="s">
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A856" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="B856" s="5" t="s">
-        <v>1498</v>
-      </c>
-    </row>
-    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A857" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="B857" s="5" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A858" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="B858" s="5" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A859" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B859" s="5" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A860" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B860" s="5" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A861" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="B861" s="5" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A862" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="B862" s="5" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A863" s="5" t="s">
-        <v>823</v>
-      </c>
-      <c r="B863" s="5" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A864" s="5" t="s">
-        <v>823</v>
-      </c>
-      <c r="B864" s="5" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A865" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="B865" s="5" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A866" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="B866" s="5" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A867" s="5" t="s">
-        <v>839</v>
-      </c>
-      <c r="B867" s="5" t="s">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="868" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A868" s="5" t="s">
-        <v>849</v>
-      </c>
-      <c r="B868" s="5" t="s">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A869" s="5" t="s">
-        <v>851</v>
-      </c>
-      <c r="B869" s="5" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A870" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="B870" s="5" t="s">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="871" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A871" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="B871" s="5" t="s">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="872" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A872" s="5" t="s">
-        <v>917</v>
-      </c>
-      <c r="B872" s="5" t="s">
-        <v>1504</v>
-      </c>
-    </row>
-    <row r="873" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A873" s="5" t="s">
-        <v>919</v>
-      </c>
-      <c r="B873" s="5" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A874" s="5" t="s">
-        <v>948</v>
-      </c>
-      <c r="B874" s="5" t="s">
-        <v>1505</v>
-      </c>
-    </row>
-    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A875" s="5" t="s">
-        <v>967</v>
-      </c>
-      <c r="B875" s="5" t="s">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="876" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A876" s="5" t="s">
-        <v>971</v>
-      </c>
-      <c r="B876" s="5" t="s">
-        <v>1507</v>
-      </c>
-    </row>
-    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A877" s="5" t="s">
-        <v>971</v>
-      </c>
-      <c r="B877" s="5" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A878" s="5" t="s">
-        <v>976</v>
-      </c>
-      <c r="B878" s="5" t="s">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A879" s="5" t="s">
-        <v>982</v>
-      </c>
-      <c r="B879" s="5" t="s">
-        <v>1509</v>
-      </c>
-    </row>
-    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A880" s="5" t="s">
-        <v>982</v>
-      </c>
-      <c r="B880" s="5" t="s">
-        <v>1509</v>
-      </c>
-    </row>
-    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A881" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="B881" s="5" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A882" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="B882" s="5" t="s">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A883" s="5" t="s">
-        <v>986</v>
-      </c>
-      <c r="B883" s="5" t="s">
-        <v>1511</v>
-      </c>
-    </row>
-    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A884" s="5" t="s">
-        <v>988</v>
-      </c>
-      <c r="B884" s="5" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A885" s="5" t="s">
-        <v>988</v>
-      </c>
-      <c r="B885" s="5" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A886" s="5" t="s">
-        <v>990</v>
-      </c>
-      <c r="B886" s="5" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A887" s="5" t="s">
-        <v>990</v>
-      </c>
-      <c r="B887" s="5" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A888" s="5" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B888" s="5" t="s">
-        <v>1513</v>
-      </c>
-    </row>
-    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A889" s="5" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B889" s="5" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A890" s="5" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B890" s="5" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A891" s="5" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B891" s="5" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A892" s="5" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B892" s="5" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A893" s="5" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B893" s="5" t="s">
-        <v>1515</v>
-      </c>
-    </row>
-    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A894" s="5" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B894" s="5" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A895" s="5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B895" s="5" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A896" s="5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B896" s="5" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A897" s="5" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B897" s="5" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A898" s="5" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B898" s="5" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A899" s="5" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B899" s="5" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A900" s="5" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B900" s="5" t="s">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A901" s="5" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B901" s="5" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A902" s="5" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B902" s="5" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A903" s="5" t="s">
-        <v>1174</v>
-      </c>
-      <c r="B903" s="5" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A904" s="5" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B904" s="5" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A905" s="5" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B905" s="5" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A906" s="5" t="s">
-        <v>1181</v>
-      </c>
-      <c r="B906" s="5" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A907" s="5" t="s">
-        <v>1183</v>
-      </c>
-      <c r="B907" s="5" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A908" s="5" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B908" s="5" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A909" s="5" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B909" s="5" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A910" s="5" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B910" s="5" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A911" s="5" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B911" s="5" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A912" s="5" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B912" s="5" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A913" s="5" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B913" s="5" t="s">
-        <v>1531</v>
-      </c>
-    </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A914" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B914" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A915" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B915" s="5" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A916" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B916" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A917" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B917" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A918" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B918" s="5" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A919" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B919" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A920" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B920" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A921" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B921" s="5" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A922" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B922" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A923" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B923" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A924" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B924" s="5" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A925" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B925" s="5" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A926" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B926" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A927" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B927" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A928" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B928" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A929" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B929" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A930" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B930" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="931" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A931" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B931" s="5" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="932" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A932" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B932" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="933" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A933" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B933" s="5" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A934" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B934" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A935" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B935" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="936" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A936" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B936" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="937" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A937" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B937" s="5" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="938" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A938" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B938" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="939" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A939" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B939" s="5" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="940" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A940" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B940" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="941" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A941" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B941" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="942" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A942" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B942" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="943" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A943" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B943" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="944" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A944" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B944" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="945" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A945" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B945" s="5" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="946" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A946" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B946" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="947" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A947" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B947" s="5" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="948" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A948" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B948" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="949" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A949" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B949" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="950" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A950" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B950" s="5" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="951" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A951" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B951" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="952" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A952" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B952" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="953" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A953" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B953" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="954" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A954" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B954" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="955" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A955" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B955" s="5" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="956" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A956" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B956" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="957" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A957" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="B957" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="958" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A958" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B958" s="5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="959" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A959" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B959" s="5" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="960" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A960" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B960" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="961" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A961" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B961" s="5" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="962" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A962" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="B962" s="5" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="963" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A963" s="5" t="s">
-        <v>1544</v>
-      </c>
-      <c r="B963" s="5" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="964" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A964" s="5" t="s">
-        <v>1544</v>
-      </c>
-      <c r="B964" s="5" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="965" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A965" s="5" t="s">
-        <v>1546</v>
-      </c>
-      <c r="B965" s="5" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="966" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A966" s="5" t="s">
-        <v>1548</v>
-      </c>
-      <c r="B966" s="5" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="967" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A967" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B967" s="5" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="968" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A968" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B968" s="5" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="969" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A969" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="B969" s="5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="970" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A970" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B970" s="5" t="s">
-        <v>1551</v>
-      </c>
-    </row>
-    <row r="971" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A971" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="B971" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="972" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A972" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B972" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="973" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A973" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B973" s="5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="974" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A974" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B974" s="5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="975" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A975" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B975" s="5" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A976" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B976" s="5" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="977" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A977" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B977" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="978" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A978" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B978" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="979" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A979" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="B979" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="980" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A980" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B980" s="5" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="981" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A981" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B981" s="5" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A982" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B982" s="5" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="983" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A983" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B983" s="5" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="984" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A984" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B984" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="985" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A985" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B985" s="5" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="986" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A986" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B986" s="5" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="987" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A987" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B987" s="5" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="988" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A988" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B988" s="5" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="989" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A989" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="B989" s="5" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="990" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A990" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="B990" s="5" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="991" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A991" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="B991" s="5" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="992" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A992" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="B992" s="5" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="993" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A993" s="5" t="s">
-        <v>702</v>
-      </c>
-      <c r="B993" s="5" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="994" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A994" s="5" t="s">
-        <v>702</v>
-      </c>
-      <c r="B994" s="5" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="995" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A995" s="5" t="s">
-        <v>718</v>
-      </c>
-      <c r="B995" s="5" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="996" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A996" s="5" t="s">
-        <v>718</v>
-      </c>
-      <c r="B996" s="5" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="997" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A997" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B997" s="5" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="998" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A998" s="5" t="s">
-        <v>731</v>
-      </c>
-      <c r="B998" s="5" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="999" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A999" s="5" t="s">
-        <v>731</v>
-      </c>
-      <c r="B999" s="5" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="1000" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1000" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="B1000" s="5" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="1001" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1001" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="B1001" s="5" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="1002" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1002" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="B1002" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="1003" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1003" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="B1003" s="5" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1004" s="5" t="s">
-        <v>772</v>
-      </c>
-      <c r="B1004" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="1005" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1005" s="5" t="s">
-        <v>772</v>
-      </c>
-      <c r="B1005" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1006" s="5" t="s">
-        <v>794</v>
-      </c>
-      <c r="B1006" s="5" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="1007" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1007" s="5" t="s">
-        <v>794</v>
-      </c>
-      <c r="B1007" s="5" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="1008" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1008" s="5" t="s">
-        <v>808</v>
-      </c>
-      <c r="B1008" s="5" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="1009" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1009" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="B1009" s="5" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="1010" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1010" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="B1010" s="5" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="1011" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1011" s="5" t="s">
-        <v>823</v>
-      </c>
-      <c r="B1011" s="5" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="1012" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1012" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="B1012" s="5" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="1013" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1013" s="5" t="s">
-        <v>837</v>
-      </c>
-      <c r="B1013" s="5" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1014" s="5" t="s">
-        <v>837</v>
-      </c>
-      <c r="B1014" s="5" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="1015" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1015" s="5" t="s">
-        <v>839</v>
-      </c>
-      <c r="B1015" s="5" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1016" s="5" t="s">
-        <v>849</v>
-      </c>
-      <c r="B1016" s="5" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1017" s="5" t="s">
-        <v>851</v>
-      </c>
-      <c r="B1017" s="5" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1018" s="5" t="s">
-        <v>889</v>
-      </c>
-      <c r="B1018" s="5" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1019" s="5" t="s">
-        <v>889</v>
-      </c>
-      <c r="B1019" s="5" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1020" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="B1020" s="5" t="s">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1021" s="5" t="s">
-        <v>917</v>
-      </c>
-      <c r="B1021" s="5" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1022" s="5" t="s">
-        <v>919</v>
-      </c>
-      <c r="B1022" s="5" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1023" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="B1023" s="5" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1024" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="B1024" s="5" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1025" s="5" t="s">
-        <v>960</v>
-      </c>
-      <c r="B1025" s="5" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1026" s="5" t="s">
-        <v>960</v>
-      </c>
-      <c r="B1026" s="5" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1027" s="5" t="s">
-        <v>962</v>
-      </c>
-      <c r="B1027" s="5" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1028" s="5" t="s">
-        <v>971</v>
-      </c>
-      <c r="B1028" s="5" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1029" s="5" t="s">
-        <v>982</v>
-      </c>
-      <c r="B1029" s="5" t="s">
-        <v>1509</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1030" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="B1030" s="5" t="s">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1031" s="5" t="s">
-        <v>986</v>
-      </c>
-      <c r="B1031" s="5" t="s">
-        <v>1511</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1032" s="5" t="s">
-        <v>988</v>
-      </c>
-      <c r="B1032" s="5" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1033" s="5" t="s">
-        <v>990</v>
-      </c>
-      <c r="B1033" s="5" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1034" s="5" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B1034" s="5" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1035" s="5" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B1035" s="5" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1036" s="5" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B1036" s="5" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="1037" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1037" s="5" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B1037" s="5" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="1038" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1038" s="5" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B1038" s="5" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1039" s="5" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B1039" s="5" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1040" s="5" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B1040" s="5" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1041" s="5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B1041" s="5" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="1042" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1042" s="5" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B1042" s="5" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="1043" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1043" s="5" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B1043" s="5" t="s">
-        <v>1161</v>
+      <c r="C629" s="1" t="s">
+        <v>1205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>